<commit_message>
@dev finish 5 interfaces
</commit_message>
<xml_diff>
--- a/PM/worklist.xlsx
+++ b/PM/worklist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{34029F3D-7E89-43DE-A3D6-653064686A99}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7DC60716-6766-4B42-8D41-3BC5C23EF24C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,10 +50,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>axios 获取用户信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>axios 修改用户信息</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -74,10 +70,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>未完成</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>axios 检验密码是否正确</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -99,6 +91,14 @@
   </si>
   <si>
     <t>ShoppingConfig</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>asyncstorage 获取用户信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -427,17 +427,18 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.25" customWidth="1"/>
-    <col min="2" max="2" width="35.375" customWidth="1"/>
-    <col min="3" max="3" width="27.375" customWidth="1"/>
+    <col min="1" max="1" width="8.21875" customWidth="1"/>
+    <col min="2" max="2" width="35.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -451,7 +452,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -462,105 +463,105 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
       <c r="D5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
       <c r="D6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
         <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
         <v>19</v>
-      </c>
-      <c r="D9" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
@dev add axios work
</commit_message>
<xml_diff>
--- a/PM/worklist.xlsx
+++ b/PM/worklist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7DC60716-6766-4B42-8D41-3BC5C23EF24C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AD1EFBC0-A06A-46F7-A4D8-C83E2585841B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -99,6 +99,14 @@
   </si>
   <si>
     <t>完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>axios 增加购物配置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AddConfig</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -424,21 +432,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.21875" customWidth="1"/>
-    <col min="2" max="2" width="35.33203125" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="8.25" customWidth="1"/>
+    <col min="2" max="2" width="35.375" customWidth="1"/>
+    <col min="3" max="3" width="27.375" customWidth="1"/>
+    <col min="5" max="5" width="8.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -452,7 +460,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -466,7 +474,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -480,7 +488,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -494,7 +502,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -508,7 +516,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -522,7 +530,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -536,7 +544,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -550,7 +558,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -562,6 +570,20 @@
       </c>
       <c r="D9" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
@dev remove nav header
</commit_message>
<xml_diff>
--- a/PM/worklist.xlsx
+++ b/PM/worklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AD1EFBC0-A06A-46F7-A4D8-C83E2585841B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8363A1B7-EA56-4BEF-A827-843178D96A34}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -107,6 +107,14 @@
   </si>
   <si>
     <t>AddConfig</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>axios 注销请求</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Setting</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -432,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -586,6 +594,20 @@
         <v>6</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
@dev: add 2 interfaces
</commit_message>
<xml_diff>
--- a/PM/worklist.xlsx
+++ b/PM/worklist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AD1EFBC0-A06A-46F7-A4D8-C83E2585841B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{19867E23-B684-436E-933C-EFB7BB7257CE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -435,18 +435,18 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.25" customWidth="1"/>
-    <col min="2" max="2" width="35.375" customWidth="1"/>
-    <col min="3" max="3" width="27.375" customWidth="1"/>
-    <col min="5" max="5" width="8.875" customWidth="1"/>
+    <col min="1" max="1" width="8.21875" customWidth="1"/>
+    <col min="2" max="2" width="35.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,7 +460,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -474,7 +474,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -488,7 +488,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -502,7 +502,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -516,7 +516,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -530,7 +530,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -541,10 +541,10 @@
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -555,10 +555,10 @@
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -572,7 +572,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>

</xml_diff>